<commit_message>
modified:   "\346\227\245\345\270\270\345\256\211\346\216\222.xlsx" 	modified:   "\346\227\245\345\270\270\350\256\260\345\275\225.docx"
</commit_message>
<xml_diff>
--- a/日常安排.xlsx
+++ b/日常安排.xlsx
@@ -1,23 +1,105 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="135" windowWidth="14805" windowHeight="7980"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211" fullCalcOnLoad="1"/>
+  <calcPr calcId="122211"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+  <si>
+    <t>日期</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>进展</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>描述</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>参考书籍</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>计算机网络</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>效率值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>计算机网络第五版，第7、8章</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.初步熟悉网络的相关知识，对IP视频
+的有关协议有一定了解，熟悉了c++的函数模板使用
+2.debug:（1）退出键（home键）
+        （2）recovery字符串调整
+        （3）布局调整，添加的通用性
+3.开发：手机遥控器</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.加密算法//depot/PDK_Release/PDK1.5.5/linux/kernel/alidrivers/modules/alidsc/ali_dsc.c
+2.//depot/ALI_SDK6.0/internal/ACAS_doc/ALi Android SDK_编程手册_安全启动.docx
+3.HDMI Dongle wifi set up</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>导师建议文档，论文初探</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">HDMI DONGLE wifi demo apk:
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">其实现协议源码：
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://code.google.com/p/google-tv-remote/
+https://code.google.com/p/boxeeremote/
+https://code.google.com/r/hafizmbilal-tvremote/
+https://code.google.com/p/tv-remote-control/
+https://code.google.com/p/second-screen-aoc/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.tomsguide.com/us/chromecast-how-to,review-1811.html
+http://hdplayer.pconline.com.cn/420/4209437_all.html
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>protocol:
+http://code.google.com/p/google-tv-pairing-protocol/
+http://code.google.com/p/anymote-protocol/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -25,13 +107,72 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -43,22 +184,75 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="yyyy/m/d"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:E5" totalsRowShown="0">
+  <autoFilter ref="A1:E5"/>
+  <tableColumns count="5">
+    <tableColumn id="1" name="日期" dataDxfId="1"/>
+    <tableColumn id="2" name="进展"/>
+    <tableColumn id="3" name="描述"/>
+    <tableColumn id="4" name="参考书籍"/>
+    <tableColumn id="5" name="效率值" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -343,37 +537,162 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="17.375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="43.875" customWidth="1"/>
+    <col min="3" max="3" width="56" customWidth="1"/>
+    <col min="4" max="4" width="74" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="81" x14ac:dyDescent="0.15">
+      <c r="A2" s="4">
+        <v>42016</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="7">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="81" x14ac:dyDescent="0.15">
+      <c r="A3" s="4">
+        <v>42017</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="8">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="67.5" x14ac:dyDescent="0.15">
+      <c r="A4" s="4">
+        <v>42017</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="8"/>
+    </row>
+    <row r="5" spans="1:5" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="A5" s="4">
+        <v>42017</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="8"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="E1:E1048576">
+    <cfRule type="iconSet" priority="4">
+      <iconSet iconSet="5Arrows">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="20"/>
+        <cfvo type="percent" val="40"/>
+        <cfvo type="percent" val="60"/>
+        <cfvo type="percent" val="80"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E5">
+    <cfRule type="iconSet" priority="2">
+      <iconSet iconSet="5Arrows">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="20"/>
+        <cfvo type="percent" val="40"/>
+        <cfvo type="percent" val="60"/>
+        <cfvo type="percent" val="80"/>
+      </iconSet>
+    </cfRule>
+    <cfRule type="iconSet" priority="1">
+      <iconSet iconSet="5Arrows">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="20"/>
+        <cfvo type="num" val="40"/>
+        <cfvo type="num" val="60"/>
+        <cfvo type="num" val="80"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="D3" r:id="rId1" display="http://www.tomsguide.com/us/chromecast-how-to,review-1811.html_x000a__x000a__x000a__x000a__x000a_"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>